<commit_message>
update solver config slightly
</commit_message>
<xml_diff>
--- a/data/data_analysis/pyrolysis_energy_balance.xlsx
+++ b/data/data_analysis/pyrolysis_energy_balance.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\natha\PycharmProjects\IAM\biochar\data\data_analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CE4022E-958C-4CBD-AE89-3179D1B564DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE31D582-496A-4E12-B644-5A54F2E879C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="0" windowWidth="14610" windowHeight="17385" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-135" yWindow="0" windowWidth="14355" windowHeight="17385" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Swine" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="379" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="379" uniqueCount="53">
   <si>
     <t>Initial Moisture Content</t>
   </si>
@@ -283,13 +283,19 @@
     <t>76% moisture content of feedstock results in a balanced system</t>
   </si>
   <si>
-    <t>74% moisture content of feedstock after mechanical separation results in a balanced system</t>
+    <t>68% moisture content of feedstock after mechanical separation results in a balanced system</t>
+  </si>
+  <si>
+    <t>72% moisture content of feedstock after mechanical separation results in a balanced system</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.0%"/>
+  </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -368,7 +374,7 @@
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -378,6 +384,7 @@
     <xf numFmtId="9" fontId="0" fillId="4" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="2" fontId="0" fillId="4" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Good" xfId="2" builtinId="26"/>
@@ -1883,8 +1890,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{23C1749D-1839-4F52-84BB-D7B762A2D609}">
   <dimension ref="A1:D33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:B33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1909,7 +1916,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="4">
-        <v>0.74</v>
+        <v>0.72</v>
       </c>
       <c r="C2" t="s">
         <v>11</v>
@@ -1929,7 +1936,7 @@
         <v>11</v>
       </c>
       <c r="D3" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -2023,7 +2030,7 @@
         <v>4</v>
       </c>
       <c r="B12" s="7">
-        <v>0.4</v>
+        <v>0.01</v>
       </c>
       <c r="C12" t="s">
         <v>6</v>
@@ -2034,7 +2041,7 @@
         <v>16</v>
       </c>
       <c r="B13" s="7">
-        <v>15.32</v>
+        <v>15.26</v>
       </c>
       <c r="C13" t="s">
         <v>15</v>
@@ -2046,7 +2053,7 @@
       </c>
       <c r="B14">
         <f>(B12*(1-B2))/(1-B3)</f>
-        <v>0.11954022988505748</v>
+        <v>3.2183908045977016E-3</v>
       </c>
       <c r="C14" t="s">
         <v>6</v>
@@ -2058,7 +2065,7 @@
       </c>
       <c r="B15">
         <f>B12-B14</f>
-        <v>0.28045977011494255</v>
+        <v>6.7816091954022986E-3</v>
       </c>
       <c r="C15" t="s">
         <v>6</v>
@@ -2080,7 +2087,7 @@
         <v>14</v>
       </c>
       <c r="B17" s="8">
-        <v>13.7</v>
+        <v>15.3</v>
       </c>
       <c r="C17" t="s">
         <v>15</v>
@@ -2095,7 +2102,7 @@
       </c>
       <c r="B18">
         <f>B16*B14</f>
-        <v>5.1414252873563222E-2</v>
+        <v>1.3842298850574714E-3</v>
       </c>
       <c r="C18" t="s">
         <v>6</v>
@@ -2118,7 +2125,7 @@
       </c>
       <c r="B21">
         <f>B13*B14*(1-B3)</f>
-        <v>1.5932800000000003</v>
+        <v>4.2728000000000009E-2</v>
       </c>
       <c r="C21" t="s">
         <v>9</v>
@@ -2130,7 +2137,7 @@
       </c>
       <c r="B22">
         <f>B21*B7</f>
-        <v>1.6145172557389906</v>
+        <v>4.3297532952911978E-2</v>
       </c>
       <c r="C22" t="s">
         <v>9</v>
@@ -2142,7 +2149,7 @@
       </c>
       <c r="B23">
         <f>B17*B18*B8</f>
-        <v>0.72619905567645715</v>
+        <v>2.183490142137804E-2</v>
       </c>
       <c r="C23" t="s">
         <v>9</v>
@@ -2197,7 +2204,7 @@
       </c>
       <c r="B27">
         <f>B22*B9</f>
-        <v>3.4770801062856654E-2</v>
+        <v>9.3247061898331688E-4</v>
       </c>
       <c r="C27" t="s">
         <v>9</v>
@@ -2209,7 +2216,7 @@
       </c>
       <c r="B28">
         <f>B22-B23</f>
-        <v>0.88831820006253348</v>
+        <v>2.1462631531533938E-2</v>
       </c>
       <c r="C28" t="s">
         <v>9</v>
@@ -2221,7 +2228,7 @@
       </c>
       <c r="B29">
         <f>B4*B15</f>
-        <v>0.75051034482758627</v>
+        <v>1.8147586206896552E-2</v>
       </c>
       <c r="C29" t="s">
         <v>9</v>
@@ -2233,7 +2240,7 @@
       </c>
       <c r="B30">
         <f>B29*B6</f>
-        <v>0.79779249655172413</v>
+        <v>1.9290884137931032E-2</v>
       </c>
       <c r="C30" t="s">
         <v>9</v>
@@ -2245,7 +2252,7 @@
       </c>
       <c r="B31">
         <f>B30*(1-B5)</f>
-        <v>7.9779249655172399E-2</v>
+        <v>1.9290884137931029E-3</v>
       </c>
       <c r="C31" t="s">
         <v>9</v>
@@ -2257,7 +2264,7 @@
       </c>
       <c r="B32" s="3">
         <f>B21-B22+B28-B29-B31-B27</f>
-        <v>2.0205487779277748E-3</v>
+        <v>-1.160466610510034E-4</v>
       </c>
       <c r="C32" t="s">
         <v>9</v>
@@ -2269,7 +2276,7 @@
       </c>
       <c r="B33" s="5">
         <f>B32/B21</f>
-        <v>1.2681692972533231E-3</v>
+        <v>-2.7159394554157313E-3</v>
       </c>
       <c r="C33" t="s">
         <v>11</v>
@@ -2285,8 +2292,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7BA2D4DE-564C-4B73-9118-5C77B92E8AFB}">
   <dimension ref="A1:D33"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2311,7 +2318,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="4">
-        <v>0.73</v>
+        <v>0.68</v>
       </c>
       <c r="C2" t="s">
         <v>11</v>
@@ -2331,7 +2338,7 @@
         <v>11</v>
       </c>
       <c r="D3" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -2425,7 +2432,7 @@
         <v>4</v>
       </c>
       <c r="B12" s="7">
-        <v>0.4</v>
+        <v>0.01</v>
       </c>
       <c r="C12" t="s">
         <v>6</v>
@@ -2436,7 +2443,7 @@
         <v>16</v>
       </c>
       <c r="B13" s="7">
-        <v>16</v>
+        <v>13.72</v>
       </c>
       <c r="C13" t="s">
         <v>15</v>
@@ -2448,7 +2455,7 @@
       </c>
       <c r="B14">
         <f>(B12*(1-B2))/(1-B3)</f>
-        <v>0.12413793103448277</v>
+        <v>3.6781609195402297E-3</v>
       </c>
       <c r="C14" t="s">
         <v>6</v>
@@ -2460,7 +2467,7 @@
       </c>
       <c r="B15">
         <f>B12-B14</f>
-        <v>0.27586206896551724</v>
+        <v>6.32183908045977E-3</v>
       </c>
       <c r="C15" t="s">
         <v>6</v>
@@ -2470,8 +2477,8 @@
       <c r="A16" t="s">
         <v>13</v>
       </c>
-      <c r="B16" s="6">
-        <v>0.47499999999999998</v>
+      <c r="B16" s="9">
+        <v>0.46500000000000002</v>
       </c>
       <c r="C16" t="s">
         <v>11</v>
@@ -2482,7 +2489,7 @@
         <v>14</v>
       </c>
       <c r="B17" s="8">
-        <v>13.7</v>
+        <v>13.75</v>
       </c>
       <c r="C17" t="s">
         <v>15</v>
@@ -2497,7 +2504,7 @@
       </c>
       <c r="B18">
         <f>B16*B14</f>
-        <v>5.8965517241379314E-2</v>
+        <v>1.710344827586207E-3</v>
       </c>
       <c r="C18" t="s">
         <v>6</v>
@@ -2520,7 +2527,7 @@
       </c>
       <c r="B21">
         <f>B13*B14*(1-B3)</f>
-        <v>1.7280000000000002</v>
+        <v>4.3903999999999999E-2</v>
       </c>
       <c r="C21" t="s">
         <v>9</v>
@@ -2532,7 +2539,7 @@
       </c>
       <c r="B22">
         <f>B21*B7</f>
-        <v>1.7510329746918154</v>
+        <v>4.4489208171799452E-2</v>
       </c>
       <c r="C22" t="s">
         <v>9</v>
@@ -2544,7 +2551,7 @@
       </c>
       <c r="B23">
         <f>B17*B18*B8</f>
-        <v>0.83285666026242233</v>
+        <v>2.4245880492550134E-2</v>
       </c>
       <c r="C23" t="s">
         <v>9</v>
@@ -2599,7 +2606,7 @@
       </c>
       <c r="B27">
         <f>B22*B9</f>
-        <v>3.7710850720913021E-2</v>
+        <v>9.5813494794616029E-4</v>
       </c>
       <c r="C27" t="s">
         <v>9</v>
@@ -2611,7 +2618,7 @@
       </c>
       <c r="B28">
         <f>B22-B23</f>
-        <v>0.91817631442939307</v>
+        <v>2.0243327679249318E-2</v>
       </c>
       <c r="C28" t="s">
         <v>9</v>
@@ -2623,7 +2630,7 @@
       </c>
       <c r="B29">
         <f>B4*B15</f>
-        <v>0.73820689655172422</v>
+        <v>1.6917241379310347E-2</v>
       </c>
       <c r="C29" t="s">
         <v>9</v>
@@ -2635,7 +2642,7 @@
       </c>
       <c r="B30">
         <f>B29*B6</f>
-        <v>0.78471393103448284</v>
+        <v>1.7983027586206898E-2</v>
       </c>
       <c r="C30" t="s">
         <v>9</v>
@@ -2647,7 +2654,7 @@
       </c>
       <c r="B31">
         <f>B30*(1-B5)</f>
-        <v>7.8471393103448264E-2</v>
+        <v>1.7983027586206894E-3</v>
       </c>
       <c r="C31" t="s">
         <v>9</v>
@@ -2659,7 +2666,7 @@
       </c>
       <c r="B32" s="3">
         <f>B21-B22+B28-B29-B31-B27</f>
-        <v>4.0754199361492362E-2</v>
+        <v>-1.5559578427331157E-5</v>
       </c>
       <c r="C32" t="s">
         <v>9</v>
@@ -2671,7 +2678,7 @@
       </c>
       <c r="B33" s="5">
         <f>B32/B21</f>
-        <v>2.3584606111974743E-2</v>
+        <v>-3.5440001884409522E-4</v>
       </c>
       <c r="C33" t="s">
         <v>11</v>

</xml_diff>